<commit_message>
tons of work on phylogenetic model
</commit_message>
<xml_diff>
--- a/data/extracted_data/raw_round1/timeseries/McGuire_etal_2025_Table2.xlsx
+++ b/data/extracted_data/raw_round1/timeseries/McGuire_etal_2025_Table2.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/hab_depuration/data/extracted_data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/hab_depuration/data/extracted_data/raw_round1/timeseries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E507A4-A93C-5A40-AEE4-308EA57AFBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224D4405-0602-7D48-ADCA-E9F35E12C7EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="4640" windowWidth="33880" windowHeight="16060" xr2:uid="{ECD6425D-59EE-2E4E-B602-BA19A8E66EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,9 +45,6 @@
     <t>day</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>phase</t>
   </si>
   <si>
@@ -69,13 +55,16 @@
   </si>
   <si>
     <t>hour</t>
+  </si>
+  <si>
+    <t>Total DST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -449,10 +438,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.83203125" bestFit="1" customWidth="1"/>
@@ -461,12 +450,12 @@
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -478,9 +467,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -496,9 +485,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -514,9 +503,9 @@
         <v>1.21313</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -532,9 +521,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>36</v>
@@ -550,9 +539,9 @@
         <v>1.769326</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>48</v>
@@ -568,9 +557,9 @@
         <v>3.850285</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -586,9 +575,9 @@
         <v>1.5257160000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -604,9 +593,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -622,9 +611,9 @@
         <v>4.2144729999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>24</v>
@@ -640,9 +629,9 @@
         <v>5.9919219999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>36</v>
@@ -658,9 +647,9 @@
         <v>10.71763</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>48</v>
@@ -676,9 +665,9 @@
         <v>13.79063</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>60</v>
@@ -694,9 +683,9 @@
         <v>5.6219460000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -712,9 +701,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -730,9 +719,9 @@
         <v>33.780290000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -748,9 +737,9 @@
         <v>51.799930000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>36</v>
@@ -766,9 +755,9 @@
         <v>84.604320000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>48</v>
@@ -784,9 +773,9 @@
         <v>25.826280000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>60</v>
@@ -802,9 +791,9 @@
         <v>17.066849999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -814,15 +803,15 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -832,15 +821,15 @@
         <v>0.5</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>39.207892999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>24</v>
@@ -850,15 +839,15 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>57.791852000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>36</v>
@@ -868,15 +857,15 @@
         <v>1.5</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>97.091275999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>48</v>
@@ -886,15 +875,15 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>43.467195000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>60</v>
@@ -904,14 +893,14 @@
         <v>2.5</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>24.214511999999999</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E19">
+  <sortState ref="B2:E19">
     <sortCondition ref="D2:D19"/>
     <sortCondition ref="C2:C19"/>
   </sortState>

</xml_diff>